<commit_message>
updated all of sanj code to latest versions
</commit_message>
<xml_diff>
--- a/Questionnaire_data/TS_advanced_mapping_v2 (1).xlsx
+++ b/Questionnaire_data/TS_advanced_mapping_v2 (1).xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjanasrinivasan/Desktop/CVD_RiskStrat_WebApp/Questionnaire_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE9E221-3AFC-E140-B68C-E3743A941CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEF84C1-A4B8-9742-99A6-C2E60C8D6DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16580" xr2:uid="{5A91DBF8-AF45-5544-993E-463958C0A548}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16640" xr2:uid="{5A91DBF8-AF45-5544-993E-463958C0A548}"/>
   </bookViews>
   <sheets>
     <sheet name="TS_advanced_mapping_v2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3766" uniqueCount="1247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3758" uniqueCount="1247">
   <si>
     <t>Category</t>
   </si>
@@ -4767,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE6F3EC-BA3F-7946-9235-F1172B103C34}">
   <dimension ref="A1:J1178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="87" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="B934" zoomScale="87" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G964" sqref="G964"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21321,7 +21334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="961" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="961" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A961" t="s">
         <v>984</v>
       </c>
@@ -21341,7 +21354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="962" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="962" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A962" t="s">
         <v>985</v>
       </c>
@@ -21361,7 +21374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="963" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="963" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A963" t="s">
         <v>986</v>
       </c>
@@ -21381,7 +21394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="964" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="964" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A964" t="s">
         <v>987</v>
       </c>
@@ -21401,7 +21414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="965" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="965" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A965" t="s">
         <v>988</v>
       </c>
@@ -21411,8 +21424,8 @@
       <c r="C965" t="s">
         <v>817</v>
       </c>
-      <c r="D965" t="s">
-        <v>3</v>
+      <c r="D965">
+        <v>2415</v>
       </c>
       <c r="E965">
         <v>2415</v>
@@ -21420,14 +21433,8 @@
       <c r="F965">
         <v>0</v>
       </c>
-      <c r="G965">
-        <v>2844</v>
-      </c>
-      <c r="H965">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="966" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="966" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A966" t="s">
         <v>990</v>
       </c>
@@ -21437,8 +21444,8 @@
       <c r="C966" t="s">
         <v>817</v>
       </c>
-      <c r="D966" t="s">
-        <v>3</v>
+      <c r="D966">
+        <v>2415</v>
       </c>
       <c r="E966">
         <v>2415</v>
@@ -21446,14 +21453,8 @@
       <c r="F966">
         <v>1</v>
       </c>
-      <c r="G966">
-        <v>2844</v>
-      </c>
-      <c r="H966">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="967" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="967" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A967" t="s">
         <v>991</v>
       </c>
@@ -21467,7 +21468,7 @@
         <v>6150</v>
       </c>
     </row>
-    <row r="968" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="968" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A968" t="s">
         <v>993</v>
       </c>
@@ -21481,7 +21482,7 @@
         <v>6150</v>
       </c>
     </row>
-    <row r="969" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="969" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A969" t="s">
         <v>994</v>
       </c>
@@ -21495,7 +21496,7 @@
         <v>6150</v>
       </c>
     </row>
-    <row r="970" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="970" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A970" t="s">
         <v>995</v>
       </c>
@@ -21509,7 +21510,7 @@
         <v>6150</v>
       </c>
     </row>
-    <row r="971" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="971" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A971" t="s">
         <v>996</v>
       </c>
@@ -21523,7 +21524,7 @@
         <v>6150</v>
       </c>
     </row>
-    <row r="972" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="972" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A972" t="s">
         <v>997</v>
       </c>
@@ -21543,7 +21544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="973" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="973" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A973" t="s">
         <v>998</v>
       </c>
@@ -21563,7 +21564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="974" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="974" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A974" t="s">
         <v>999</v>
       </c>
@@ -21583,7 +21584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="975" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="975" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A975" t="s">
         <v>1000</v>
       </c>
@@ -21603,7 +21604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="976" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="976" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A976" t="s">
         <v>1001</v>
       </c>
@@ -22529,7 +22530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1025" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1025" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1025" t="s">
         <v>1050</v>
       </c>
@@ -22549,7 +22550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1026" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1026" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1026" t="s">
         <v>1051</v>
       </c>
@@ -22569,7 +22570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1027" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1027" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1027" t="s">
         <v>1052</v>
       </c>
@@ -22589,7 +22590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1028" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1028" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1028" t="s">
         <v>1053</v>
       </c>
@@ -22603,7 +22604,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="1029" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1029" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1029" t="s">
         <v>1054</v>
       </c>
@@ -22617,7 +22618,7 @@
         <v>2473</v>
       </c>
     </row>
-    <row r="1030" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1030" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1030" t="s">
         <v>1055</v>
       </c>
@@ -22627,23 +22628,17 @@
       <c r="C1030" t="s">
         <v>817</v>
       </c>
-      <c r="D1030" t="s">
-        <v>3</v>
+      <c r="D1030">
+        <v>6177</v>
       </c>
       <c r="E1030">
-        <v>6153</v>
+        <v>6177</v>
       </c>
       <c r="F1030">
         <v>-7</v>
       </c>
-      <c r="G1030">
-        <v>6177</v>
-      </c>
-      <c r="H1030">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="1031" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1031" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1031" t="s">
         <v>1057</v>
       </c>
@@ -22653,17 +22648,11 @@
       <c r="C1031" t="s">
         <v>817</v>
       </c>
-      <c r="D1031" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1031">
-        <v>6153</v>
-      </c>
-      <c r="F1031">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D1031">
+        <v>6177</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1032" t="s">
         <v>1058</v>
       </c>
@@ -22673,17 +22662,11 @@
       <c r="C1032" t="s">
         <v>817</v>
       </c>
-      <c r="D1032" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1032">
-        <v>6153</v>
-      </c>
-      <c r="F1032">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D1032">
+        <v>6177</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1033" t="s">
         <v>1059</v>
       </c>
@@ -22693,23 +22676,17 @@
       <c r="C1033" t="s">
         <v>817</v>
       </c>
-      <c r="D1033" t="s">
-        <v>3</v>
+      <c r="D1033">
+        <v>6177</v>
       </c>
       <c r="E1033">
-        <v>6153</v>
+        <v>6177</v>
       </c>
       <c r="F1033">
         <v>1</v>
       </c>
-      <c r="G1033">
-        <v>6177</v>
-      </c>
-      <c r="H1033">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1034" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1034" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1034" t="s">
         <v>1060</v>
       </c>
@@ -22719,23 +22696,17 @@
       <c r="C1034" t="s">
         <v>817</v>
       </c>
-      <c r="D1034" t="s">
-        <v>3</v>
+      <c r="D1034">
+        <v>6177</v>
       </c>
       <c r="E1034">
-        <v>6153</v>
+        <v>6177</v>
       </c>
       <c r="F1034">
         <v>2</v>
       </c>
-      <c r="G1034">
-        <v>6177</v>
-      </c>
-      <c r="H1034">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1035" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1035" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1035" t="s">
         <v>1061</v>
       </c>
@@ -22745,23 +22716,17 @@
       <c r="C1035" t="s">
         <v>817</v>
       </c>
-      <c r="D1035" t="s">
-        <v>3</v>
+      <c r="D1035">
+        <v>6177</v>
       </c>
       <c r="E1035">
-        <v>6153</v>
+        <v>6177</v>
       </c>
       <c r="F1035">
         <v>3</v>
       </c>
-      <c r="G1035">
-        <v>6177</v>
-      </c>
-      <c r="H1035">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1036" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="1036" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1036" t="s">
         <v>1062</v>
       </c>
@@ -22775,7 +22740,7 @@
         <v>2492</v>
       </c>
     </row>
-    <row r="1037" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1037" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1037" t="s">
         <v>1063</v>
       </c>
@@ -22789,7 +22754,7 @@
         <v>2492</v>
       </c>
     </row>
-    <row r="1038" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1038" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1038" t="s">
         <v>1064</v>
       </c>
@@ -22803,7 +22768,7 @@
         <v>6154</v>
       </c>
     </row>
-    <row r="1039" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1039" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1039" t="s">
         <v>1065</v>
       </c>
@@ -22817,7 +22782,7 @@
         <v>6154</v>
       </c>
     </row>
-    <row r="1040" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1040" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1040" t="s">
         <v>1066</v>
       </c>

</xml_diff>